<commit_message>
to do wouter don 28/03-a
</commit_message>
<xml_diff>
--- a/To Do/Wouter Peeters.xlsx
+++ b/To Do/Wouter Peeters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
   <si>
     <t>Prioriteit:</t>
   </si>
@@ -121,9 +121,6 @@
     <t>3 uur</t>
   </si>
   <si>
-    <t>3uur</t>
-  </si>
-  <si>
     <t>sql Stored procedures</t>
   </si>
   <si>
@@ -146,6 +143,12 @@
   </si>
   <si>
     <t>sql</t>
+  </si>
+  <si>
+    <t>4uur</t>
+  </si>
+  <si>
+    <t>helpen trigger</t>
   </si>
 </sst>
 </file>
@@ -263,371 +266,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="41">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -851,7 +490,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -944,14 +583,14 @@
     <sortCondition descending="1" ref="G1:G200"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="Opmerking" dataDxfId="33"/>
+    <tableColumn id="1" name="Opmerking" dataDxfId="2"/>
     <tableColumn id="2" name="Geschatte tijd"/>
     <tableColumn id="5" name="Werkelijke tijd"/>
     <tableColumn id="9" name="Voltooid"/>
     <tableColumn id="6" name="Prioriteit"/>
-    <tableColumn id="3" name="Deelnemers" dataDxfId="32"/>
+    <tableColumn id="3" name="Deelnemers" dataDxfId="1"/>
     <tableColumn id="4" name="Solved"/>
-    <tableColumn id="8" name="APP" dataDxfId="31"/>
+    <tableColumn id="8" name="APP" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1312,7 +951,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2" t="s">
         <v>0</v>
@@ -1341,7 +980,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I3" t="s">
         <v>1</v>
@@ -1421,7 +1060,7 @@
         <v>7</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I6" s="11">
         <f>COUNTIFS(G2:G38,"Not Started")</f>
@@ -1443,7 +1082,7 @@
         <v>34</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D7" s="23">
         <v>41358</v>
@@ -1460,11 +1099,11 @@
       <c r="H7" s="2"/>
       <c r="I7" s="12">
         <f>COUNTIFS(G2:G38,"In Process")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="13">
         <f>I7/$I$10</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K7" s="16" t="s">
         <v>12</v>
@@ -1472,13 +1111,13 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="23">
         <v>41361</v>
@@ -1493,7 +1132,7 @@
         <v>7</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I8" s="10">
         <f>COUNTIFS(G2:G38,"Fixed")</f>
@@ -1509,13 +1148,13 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="23">
         <v>41361</v>
@@ -1536,7 +1175,7 @@
       </c>
       <c r="J9" s="18">
         <f>I9/$I$10</f>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="K9" s="19" t="s">
         <v>4</v>
@@ -1544,13 +1183,13 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="23">
         <v>41361</v>
@@ -1567,7 +1206,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="20">
         <f>SUM(I6:I9)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J10" s="21">
         <v>1</v>
@@ -1577,12 +1216,30 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="E11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="23">
+        <v>41361</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -1844,27 +1501,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G41">
-    <cfRule type="cellIs" dxfId="40" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="22" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="23" operator="equal">
       <formula>"In Process"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="24" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:H1048576">
-    <cfRule type="expression" dxfId="37" priority="15">
+    <cfRule type="expression" dxfId="6" priority="15">
       <formula>$G1="Solved"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="16">
+    <cfRule type="expression" dxfId="5" priority="16">
       <formula>$G1="Not Started"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="17">
+    <cfRule type="expression" dxfId="4" priority="17">
       <formula>$G1="In Process"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="18">
+    <cfRule type="expression" dxfId="3" priority="18">
       <formula>$G1="Fixed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
yea het werkt eindelijk
</commit_message>
<xml_diff>
--- a/To Do/Wouter Peeters.xlsx
+++ b/To Do/Wouter Peeters.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="ToDO" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" iterateDelta="1E-4"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="53">
   <si>
     <t>Prioriteit:</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>6 uur</t>
+  </si>
+  <si>
+    <t>7 uur</t>
+  </si>
+  <si>
+    <t>festivals aanpassen afmaken</t>
   </si>
 </sst>
 </file>
@@ -284,7 +290,148 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -508,13 +655,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -534,7 +681,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -601,14 +747,14 @@
     <sortCondition descending="1" ref="G1:G200"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="Opmerking" dataDxfId="2"/>
+    <tableColumn id="1" name="Opmerking" dataDxfId="14"/>
     <tableColumn id="2" name="Geschatte tijd"/>
     <tableColumn id="5" name="Werkelijke tijd"/>
     <tableColumn id="9" name="Voltooid"/>
     <tableColumn id="6" name="Prioriteit"/>
-    <tableColumn id="3" name="Deelnemers" dataDxfId="1"/>
+    <tableColumn id="3" name="Deelnemers" dataDxfId="13"/>
     <tableColumn id="4" name="Solved"/>
-    <tableColumn id="8" name="APP" dataDxfId="0"/>
+    <tableColumn id="8" name="APP" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -904,7 +1050,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,11 +1263,11 @@
       <c r="H7" s="2"/>
       <c r="I7" s="12">
         <f>COUNTIFS(G2:G38,"In Process")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" s="13">
         <f>I7/$I$10</f>
-        <v>0.14285714285714285</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="K7" s="16" t="s">
         <v>12</v>
@@ -1189,11 +1335,11 @@
       <c r="H9" s="2"/>
       <c r="I9" s="17">
         <f>COUNTIFS(A2:G2038,"Solved")</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J9" s="18">
         <f>I9/$I$10</f>
-        <v>0.8571428571428571</v>
+        <v>0.93333333333333335</v>
       </c>
       <c r="K9" s="19" t="s">
         <v>4</v>
@@ -1224,7 +1370,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="20">
         <f>SUM(I6:I9)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J10" s="21">
         <v>1</v>
@@ -1367,7 +1513,7 @@
         <v>21</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" t="s">
@@ -1378,11 +1524,27 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="E16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="A16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="23">
+        <v>41009</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1587,27 +1749,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G41">
-    <cfRule type="cellIs" dxfId="9" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
       <formula>"In Process"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="24" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:H1048576">
-    <cfRule type="expression" dxfId="6" priority="15">
+    <cfRule type="expression" dxfId="18" priority="15">
       <formula>$G1="Solved"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="16">
+    <cfRule type="expression" dxfId="17" priority="16">
       <formula>$G1="Not Started"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="17">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>$G1="In Process"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="18">
+    <cfRule type="expression" dxfId="15" priority="18">
       <formula>$G1="Fixed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>